<commit_message>
update datasets to involve ptdf
</commit_message>
<xml_diff>
--- a/spine_rts-gmlc/datasets/storage.xlsx
+++ b/spine_rts-gmlc/datasets/storage.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="storage" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="117">
   <si>
     <t>GEN UID</t>
   </si>
@@ -59,12 +59,6 @@
     <t>313_TAIL_STORAGE</t>
   </si>
   <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>parameter</t>
-  </si>
-  <si>
     <t>obj_name</t>
   </si>
   <si>
@@ -83,9 +77,6 @@
     <t>unit</t>
   </si>
   <si>
-    <t>parameter_name</t>
-  </si>
-  <si>
     <t>commodity</t>
   </si>
   <si>
@@ -377,7 +368,13 @@
     <t>RES_gen-322_HYDRO_4</t>
   </si>
   <si>
-    <t>node_has_state_true</t>
+    <t>parameter_names</t>
+  </si>
+  <si>
+    <t>parameter_values</t>
+  </si>
+  <si>
+    <t>value_true</t>
   </si>
 </sst>
 </file>
@@ -1274,7 +1271,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C1" sqref="C1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1288,27 +1285,27 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>114</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D2">
         <v>150</v>
@@ -1316,13 +1313,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D3">
         <v>1200</v>
@@ -1330,36 +1327,36 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G4">
         <v>75</v>
       </c>
       <c r="H4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1376,65 +1373,66 @@
   <dimension ref="A1:D87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="25.54296875" customWidth="1"/>
+    <col min="3" max="3" width="9.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>114</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
@@ -1442,13 +1440,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
@@ -1456,13 +1454,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
@@ -1470,13 +1468,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D8" t="b">
         <v>0</v>
@@ -1484,13 +1482,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D9" t="b">
         <v>0</v>
@@ -1498,13 +1496,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D10" t="b">
         <v>0</v>
@@ -1512,13 +1510,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
@@ -1526,13 +1524,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
@@ -1540,13 +1538,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
@@ -1554,13 +1552,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D14" t="b">
         <v>0</v>
@@ -1568,13 +1566,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D15" t="b">
         <v>0</v>
@@ -1582,13 +1580,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
@@ -1596,13 +1594,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D17" t="b">
         <v>0</v>
@@ -1610,13 +1608,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D18" t="b">
         <v>0</v>
@@ -1624,13 +1622,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D19" t="b">
         <v>0</v>
@@ -1638,13 +1636,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D20" t="b">
         <v>0</v>
@@ -1652,13 +1650,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D21" t="b">
         <v>0</v>
@@ -1666,13 +1664,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D22" t="b">
         <v>0</v>
@@ -1680,13 +1678,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D23" t="b">
         <v>0</v>
@@ -1694,13 +1692,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D24" t="b">
         <v>0</v>
@@ -1708,13 +1706,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C25" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D25" t="b">
         <v>0</v>
@@ -1722,13 +1720,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D26" t="b">
         <v>0</v>
@@ -1736,13 +1734,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D27" t="b">
         <v>0</v>
@@ -1750,13 +1748,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C28" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D28" t="b">
         <v>0</v>
@@ -1764,13 +1762,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C29" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D29" t="b">
         <v>0</v>
@@ -1778,13 +1776,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C30" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D30" t="b">
         <v>0</v>
@@ -1792,13 +1790,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C31" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D31" t="b">
         <v>0</v>
@@ -1806,13 +1804,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C32" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D32" t="b">
         <v>0</v>
@@ -1820,13 +1818,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C33" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D33" t="b">
         <v>0</v>
@@ -1834,13 +1832,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B34" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C34" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D34" t="b">
         <v>0</v>
@@ -1848,13 +1846,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C35" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D35" t="b">
         <v>0</v>
@@ -1862,13 +1860,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C36" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D36" t="b">
         <v>0</v>
@@ -1876,13 +1874,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B37" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C37" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D37" t="b">
         <v>0</v>
@@ -1890,13 +1888,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B38" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C38" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D38" t="b">
         <v>0</v>
@@ -1904,13 +1902,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B39" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C39" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D39" t="b">
         <v>0</v>
@@ -1918,13 +1916,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B40" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C40" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D40" t="b">
         <v>0</v>
@@ -1932,13 +1930,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B41" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C41" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D41" t="b">
         <v>0</v>
@@ -1946,13 +1944,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B42" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C42" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D42" t="b">
         <v>0</v>
@@ -1960,13 +1958,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B43" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C43" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D43" t="b">
         <v>0</v>
@@ -1974,13 +1972,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B44" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C44" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D44" t="b">
         <v>0</v>
@@ -1988,13 +1986,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B45" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C45" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D45" t="b">
         <v>0</v>
@@ -2002,13 +2000,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B46" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C46" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D46" t="b">
         <v>0</v>
@@ -2016,13 +2014,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B47" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C47" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D47" t="b">
         <v>0</v>
@@ -2030,13 +2028,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B48" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C48" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D48" t="b">
         <v>0</v>
@@ -2044,13 +2042,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B49" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C49" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D49" t="b">
         <v>0</v>
@@ -2058,13 +2056,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B50" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C50" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D50" t="b">
         <v>0</v>
@@ -2072,13 +2070,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B51" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C51" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D51" t="b">
         <v>0</v>
@@ -2086,13 +2084,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B52" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C52" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D52" t="b">
         <v>0</v>
@@ -2100,13 +2098,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B53" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C53" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D53" t="b">
         <v>0</v>
@@ -2114,13 +2112,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B54" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C54" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D54" t="b">
         <v>0</v>
@@ -2128,13 +2126,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B55" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C55" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D55" t="b">
         <v>0</v>
@@ -2142,13 +2140,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B56" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C56" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D56" t="b">
         <v>0</v>
@@ -2156,13 +2154,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B57" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C57" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D57" t="b">
         <v>0</v>
@@ -2170,13 +2168,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B58" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C58" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D58" t="b">
         <v>0</v>
@@ -2184,13 +2182,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B59" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C59" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D59" t="b">
         <v>0</v>
@@ -2198,13 +2196,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B60" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C60" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D60" t="b">
         <v>0</v>
@@ -2212,13 +2210,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B61" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C61" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D61" t="b">
         <v>0</v>
@@ -2226,13 +2224,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B62" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C62" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D62" t="b">
         <v>0</v>
@@ -2240,13 +2238,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B63" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C63" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D63" t="b">
         <v>0</v>
@@ -2254,13 +2252,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B64" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C64" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D64" t="b">
         <v>0</v>
@@ -2268,13 +2266,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B65" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C65" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D65" t="b">
         <v>0</v>
@@ -2282,13 +2280,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B66" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C66" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D66" t="b">
         <v>0</v>
@@ -2296,13 +2294,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B67" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C67" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D67" t="b">
         <v>0</v>
@@ -2310,13 +2308,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B68" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C68" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D68" t="b">
         <v>0</v>
@@ -2324,13 +2322,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B69" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C69" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D69" t="b">
         <v>0</v>
@@ -2338,13 +2336,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B70" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C70" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D70" t="b">
         <v>0</v>
@@ -2352,13 +2350,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B71" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C71" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D71" t="b">
         <v>0</v>
@@ -2366,13 +2364,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B72" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C72" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D72" t="b">
         <v>0</v>
@@ -2380,13 +2378,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B73" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C73" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D73" t="b">
         <v>0</v>
@@ -2394,13 +2392,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B74" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C74" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D74" t="b">
         <v>0</v>
@@ -2408,13 +2406,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B75" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C75" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D75" t="b">
         <v>0</v>
@@ -2422,13 +2420,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B76" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C76" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D76" t="b">
         <v>0</v>
@@ -2436,13 +2434,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B77" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C77" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D77" t="b">
         <v>0</v>
@@ -2450,13 +2448,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B78" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C78" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D78" t="b">
         <v>0</v>
@@ -2464,13 +2462,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B79" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C79" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D79" t="b">
         <v>0</v>
@@ -2478,13 +2476,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B80" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C80" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D80" t="b">
         <v>0</v>
@@ -2492,13 +2490,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B81" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C81" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D81" t="b">
         <v>0</v>
@@ -2506,13 +2504,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B82" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C82" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D82" t="b">
         <v>0</v>
@@ -2520,13 +2518,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B83" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C83" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D83" t="b">
         <v>0</v>
@@ -2534,13 +2532,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B84" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C84" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D84" t="b">
         <v>0</v>
@@ -2548,13 +2546,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B85" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C85" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D85" t="b">
         <v>0</v>
@@ -2562,13 +2560,13 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B86" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C86" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D86" t="b">
         <v>0</v>
@@ -2576,13 +2574,13 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B87" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C87" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D87" t="b">
         <v>0</v>
@@ -2598,7 +2596,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E1" sqref="E1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2613,53 +2611,53 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>114</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>115</v>
       </c>
       <c r="H1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -2668,16 +2666,16 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F3">
         <v>0.85</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2691,7 +2689,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E1" sqref="E1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2706,48 +2704,48 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>114</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>115</v>
       </c>
       <c r="H1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I2" t="str">
         <f>CONCATENATE("bus-",LEFT(D2,3))</f>
@@ -2756,7 +2754,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -2765,16 +2763,16 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F3">
         <v>0.85</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I3" t="str">
         <f>CONCATENATE("bus-",LEFT(C3,3))</f>
@@ -2803,24 +2801,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
         <v>17</v>
-      </c>
-      <c r="B1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>